<commit_message>
novas redes/ começo do qqplot
</commit_message>
<xml_diff>
--- a/Peaks-dataset-article/redes-ensemble-s/Teste01/content/results/metrics_11_7.xlsx
+++ b/Peaks-dataset-article/redes-ensemble-s/Teste01/content/results/metrics_11_7.xlsx
@@ -518,1376 +518,1376 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_7</t>
+          <t>model_11_7_16</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9350826468985746</v>
+        <v>0.950049199157486</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7929678889776525</v>
+        <v>0.742422213860165</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9209388073495474</v>
+        <v>0.9463198220808697</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9609511516787761</v>
+        <v>0.6678865670081366</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9454540868948099</v>
+        <v>0.9239201112557842</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4341026391061575</v>
+        <v>0.3340212352361806</v>
       </c>
       <c r="H2" t="n">
-        <v>1.384424679701653</v>
+        <v>1.722423841953726</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3133049351950845</v>
+        <v>0.7345316529290643</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2125695799047683</v>
+        <v>0.4068587203137579</v>
       </c>
       <c r="K2" t="n">
-        <v>0.2629372575499264</v>
+        <v>0.5706951866214111</v>
       </c>
       <c r="L2" t="n">
-        <v>1.757077478411768</v>
+        <v>0.7029155086039656</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6588646591722441</v>
+        <v>0.5779457026712636</v>
       </c>
       <c r="N2" t="n">
-        <v>1.311603294886842</v>
+        <v>1.239763844044067</v>
       </c>
       <c r="O2" t="n">
-        <v>0.6869138917510738</v>
+        <v>0.6025500477465143</v>
       </c>
       <c r="P2" t="n">
-        <v>59.66894855441222</v>
+        <v>60.19310141895006</v>
       </c>
       <c r="Q2" t="n">
-        <v>95.01634747559004</v>
+        <v>95.54050034012786</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_8</t>
+          <t>model_11_7_17</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9351436961854332</v>
+        <v>0.9501148397108446</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7929300605127437</v>
+        <v>0.7424163520422027</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9190268108462849</v>
+        <v>0.9459637321556906</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9549197786338502</v>
+        <v>0.6587075384040166</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9412626151232945</v>
+        <v>0.9228457983252656</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4336944022438275</v>
+        <v>0.3335822965536239</v>
       </c>
       <c r="H3" t="n">
-        <v>1.384677638820682</v>
+        <v>1.72246303995743</v>
       </c>
       <c r="I3" t="n">
-        <v>0.320881824949282</v>
+        <v>0.7394042023778988</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2454024671608055</v>
+        <v>0.4181035766206908</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2831421460550438</v>
+        <v>0.5787538894992947</v>
       </c>
       <c r="L3" t="n">
-        <v>1.7651424661423</v>
+        <v>0.7023898063637387</v>
       </c>
       <c r="M3" t="n">
-        <v>0.6585547830240303</v>
+        <v>0.5775658374190979</v>
       </c>
       <c r="N3" t="n">
-        <v>1.31131025830992</v>
+        <v>1.239448769387946</v>
       </c>
       <c r="O3" t="n">
-        <v>0.6865908235336984</v>
+        <v>0.6021540108441346</v>
       </c>
       <c r="P3" t="n">
-        <v>59.67083027040336</v>
+        <v>60.19573135558103</v>
       </c>
       <c r="Q3" t="n">
-        <v>95.01822919158118</v>
+        <v>95.54313027675884</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_6</t>
+          <t>model_11_7_15</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.934844113300594</v>
+        <v>0.9499684459701297</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7927933507258413</v>
+        <v>0.74241500541617</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9217107573683391</v>
+        <v>0.9466736826961015</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9666162978838269</v>
+        <v>0.6768890924068289</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9489701671308973</v>
+        <v>0.92497797817723</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4356977143741994</v>
+        <v>0.3345612321718655</v>
       </c>
       <c r="H4" t="n">
-        <v>1.38559181779519</v>
+        <v>1.722472044851912</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3102458395439386</v>
+        <v>0.7296896081988058</v>
       </c>
       <c r="J4" t="n">
-        <v>0.1817303157349155</v>
+        <v>0.3958300909376201</v>
       </c>
       <c r="K4" t="n">
-        <v>0.2459880776394271</v>
+        <v>0.5627598495682129</v>
       </c>
       <c r="L4" t="n">
-        <v>1.748259918874093</v>
+        <v>0.7034163159591106</v>
       </c>
       <c r="M4" t="n">
-        <v>0.6600740218901205</v>
+        <v>0.5784126832736861</v>
       </c>
       <c r="N4" t="n">
-        <v>1.312748256157149</v>
+        <v>1.240151459343377</v>
       </c>
       <c r="O4" t="n">
-        <v>0.6881747395435762</v>
+        <v>0.6030369086799652</v>
       </c>
       <c r="P4" t="n">
-        <v>59.66161318348611</v>
+        <v>60.1898707206926</v>
       </c>
       <c r="Q4" t="n">
-        <v>95.00901210466392</v>
+        <v>95.53726964187041</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_9</t>
+          <t>model_11_7_18</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9350329433606258</v>
+        <v>0.9501660054295274</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7926845223916363</v>
+        <v>0.7423979718337466</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9159111662023017</v>
+        <v>0.9456057499695555</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9486080958461541</v>
+        <v>0.649363403244214</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9364181213777022</v>
+        <v>0.9217562774158299</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4344350068932845</v>
+        <v>0.333240151157196</v>
       </c>
       <c r="H5" t="n">
-        <v>1.386319553367127</v>
+        <v>1.72258594849601</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3332285504482235</v>
+        <v>0.7443026445421026</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2797612720002171</v>
+        <v>0.4295506982842376</v>
       </c>
       <c r="K5" t="n">
-        <v>0.3064949112242203</v>
+        <v>0.58692667141317</v>
       </c>
       <c r="L5" t="n">
-        <v>1.772499186145917</v>
+        <v>0.7018439996967568</v>
       </c>
       <c r="M5" t="n">
-        <v>0.659116838575138</v>
+        <v>0.5772695654174018</v>
       </c>
       <c r="N5" t="n">
-        <v>1.311841871868996</v>
+        <v>1.239203173938268</v>
       </c>
       <c r="O5" t="n">
-        <v>0.6871768069532321</v>
+        <v>0.6018451259299586</v>
       </c>
       <c r="P5" t="n">
-        <v>59.66741785367687</v>
+        <v>60.19778374855387</v>
       </c>
       <c r="Q5" t="n">
-        <v>95.01481677485469</v>
+        <v>95.54518266973169</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_5</t>
+          <t>model_11_7_14</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9344235174460603</v>
+        <v>0.9498721332203904</v>
       </c>
       <c r="C6" t="n">
-        <v>0.7924029999699304</v>
+        <v>0.74239414383728</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9214028721555386</v>
+        <v>0.9470255542658768</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9718403420528515</v>
+        <v>0.6857019592826958</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9517933273973157</v>
+        <v>0.9260185440073436</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4385102407901325</v>
+        <v>0.3352052759728521</v>
       </c>
       <c r="H6" t="n">
-        <v>1.388202095097366</v>
+        <v>1.722611546326008</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3114659318978507</v>
+        <v>0.7248747805327128</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1532922715375928</v>
+        <v>0.3850338045389952</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2323791017177218</v>
+        <v>0.5549542925358539</v>
       </c>
       <c r="L6" t="n">
-        <v>1.73884198075221</v>
+        <v>0.7038927905746791</v>
       </c>
       <c r="M6" t="n">
-        <v>0.6622010576782043</v>
+        <v>0.5789691494137249</v>
       </c>
       <c r="N6" t="n">
-        <v>1.31476711625891</v>
+        <v>1.240613760542126</v>
       </c>
       <c r="O6" t="n">
-        <v>0.6903923276487297</v>
+        <v>0.603617064735629</v>
       </c>
       <c r="P6" t="n">
-        <v>59.64874422660638</v>
+        <v>60.18602434144453</v>
       </c>
       <c r="Q6" t="n">
-        <v>94.9961431477842</v>
+        <v>95.53342326262235</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_10</t>
+          <t>model_11_7_19</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9347579617720109</v>
+        <v>0.9502033489210344</v>
       </c>
       <c r="C7" t="n">
-        <v>0.7922377933722244</v>
+        <v>0.7423675454378331</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9115355134303194</v>
+        <v>0.9452459624700371</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9421118350731628</v>
+        <v>0.6398679968014187</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9309514936010416</v>
+        <v>0.920652757575871</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4362738100425262</v>
+        <v>0.3329904350575373</v>
       </c>
       <c r="H7" t="n">
-        <v>1.389306832376932</v>
+        <v>1.722789409945584</v>
       </c>
       <c r="I7" t="n">
-        <v>0.3505684559341328</v>
+        <v>0.749225789676282</v>
       </c>
       <c r="J7" t="n">
-        <v>0.315124861013316</v>
+        <v>0.4411831362719819</v>
       </c>
       <c r="K7" t="n">
-        <v>0.3328466584737245</v>
+        <v>0.5952044629741318</v>
       </c>
       <c r="L7" t="n">
-        <v>1.778870011964315</v>
+        <v>0.7012810439647008</v>
       </c>
       <c r="M7" t="n">
-        <v>0.6605102649032233</v>
+        <v>0.577053234162618</v>
       </c>
       <c r="N7" t="n">
-        <v>1.313161783494348</v>
+        <v>1.239023925179035</v>
       </c>
       <c r="O7" t="n">
-        <v>0.6886295543248943</v>
+        <v>0.6016195850057913</v>
       </c>
       <c r="P7" t="n">
-        <v>59.65897045612166</v>
+        <v>60.19928302593032</v>
       </c>
       <c r="Q7" t="n">
-        <v>95.00636937729948</v>
+        <v>95.54668194710814</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_4</t>
+          <t>model_11_7_13</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9338173873805012</v>
+        <v>0.9497592969783316</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7917945366112633</v>
+        <v>0.7423590269592055</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9200691803475409</v>
+        <v>0.9473748353033625</v>
       </c>
       <c r="E8" t="n">
-        <v>0.976559793263884</v>
+        <v>0.694308746568348</v>
       </c>
       <c r="F8" t="n">
-        <v>0.953909925994191</v>
+        <v>0.9270399192495582</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4425634353294979</v>
+        <v>0.3359598124430623</v>
       </c>
       <c r="H8" t="n">
-        <v>1.392270892378489</v>
+        <v>1.722846373051391</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3167511067284703</v>
+        <v>0.7200954003639715</v>
       </c>
       <c r="J8" t="n">
-        <v>0.1276010718110962</v>
+        <v>0.3744899779026937</v>
       </c>
       <c r="K8" t="n">
-        <v>0.2221760892697833</v>
+        <v>0.5472926891333325</v>
       </c>
       <c r="L8" t="n">
-        <v>1.728954140201254</v>
+        <v>0.7043506855086288</v>
       </c>
       <c r="M8" t="n">
-        <v>0.6652544139872338</v>
+        <v>0.5796204037497837</v>
       </c>
       <c r="N8" t="n">
-        <v>1.317676540573594</v>
+        <v>1.241155374504008</v>
       </c>
       <c r="O8" t="n">
-        <v>0.6935756716571535</v>
+        <v>0.6042960443170563</v>
       </c>
       <c r="P8" t="n">
-        <v>59.63034293626382</v>
+        <v>60.181527463993</v>
       </c>
       <c r="Q8" t="n">
-        <v>94.97774185744163</v>
+        <v>95.52892638517081</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_11</t>
+          <t>model_11_7_20</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.9343297462293279</v>
+        <v>0.9502273870690752</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7915997314047898</v>
+        <v>0.7423256223566013</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9058631350419656</v>
+        <v>0.9448845473540121</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9355369164998857</v>
+        <v>0.6302319510813021</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9249074463982394</v>
+        <v>0.9195362690554427</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4391372893481988</v>
+        <v>0.3328296918509035</v>
       </c>
       <c r="H9" t="n">
-        <v>1.393573555691173</v>
+        <v>1.723069749782819</v>
       </c>
       <c r="I9" t="n">
-        <v>0.3730470460462567</v>
+        <v>0.7541712062687402</v>
       </c>
       <c r="J9" t="n">
-        <v>0.3509166382133091</v>
+        <v>0.4529878657442389</v>
       </c>
       <c r="K9" t="n">
-        <v>0.3619818421297829</v>
+        <v>0.6035795360064895</v>
       </c>
       <c r="L9" t="n">
-        <v>1.786964763724666</v>
+        <v>0.7006985615987245</v>
       </c>
       <c r="M9" t="n">
-        <v>0.6626743463785201</v>
+        <v>0.5769139379932708</v>
       </c>
       <c r="N9" t="n">
-        <v>1.315217218099226</v>
+        <v>1.238908542068439</v>
       </c>
       <c r="O9" t="n">
-        <v>0.6908857652288606</v>
+        <v>0.6014743587101321</v>
       </c>
       <c r="P9" t="n">
-        <v>59.64588636559395</v>
+        <v>60.20024871142561</v>
       </c>
       <c r="Q9" t="n">
-        <v>94.99328528677175</v>
+        <v>95.54764763260343</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_3</t>
+          <t>model_11_7_12</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9330225063753058</v>
+        <v>0.9496295350128591</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7909662830539388</v>
+        <v>0.7423090692513823</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9177523873905186</v>
+        <v>0.9477216396215382</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9807220646749009</v>
+        <v>0.7026981369681649</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9553078238374632</v>
+        <v>0.9280412835750528</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4478788082713304</v>
+        <v>0.3368275313036764</v>
       </c>
       <c r="H10" t="n">
-        <v>1.397809427730075</v>
+        <v>1.723180440473639</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3259321302233917</v>
+        <v>0.7153499103349286</v>
       </c>
       <c r="J10" t="n">
-        <v>0.1049429826912544</v>
+        <v>0.3642124753893712</v>
       </c>
       <c r="K10" t="n">
-        <v>0.2154375564573231</v>
+        <v>0.5397811928621499</v>
       </c>
       <c r="L10" t="n">
-        <v>1.718723201628291</v>
+        <v>0.7047831071982489</v>
       </c>
       <c r="M10" t="n">
-        <v>0.6692374827154636</v>
+        <v>0.5803684444416981</v>
       </c>
       <c r="N10" t="n">
-        <v>1.321491969398532</v>
+        <v>1.241778231938276</v>
       </c>
       <c r="O10" t="n">
-        <v>0.6977283078672329</v>
+        <v>0.6050759306498832</v>
       </c>
       <c r="P10" t="n">
-        <v>59.60646520083008</v>
+        <v>60.17636851235809</v>
       </c>
       <c r="Q10" t="n">
-        <v>94.95386412200789</v>
+        <v>95.52376743353591</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_12</t>
+          <t>model_11_7_21</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.933763766030976</v>
+        <v>0.9502386060289226</v>
       </c>
       <c r="C11" t="n">
-        <v>0.7907842034474895</v>
+        <v>0.7422726736573397</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8988961955768071</v>
+        <v>0.9445215629083853</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9289966951805932</v>
+        <v>0.6204659859353165</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9183508744760319</v>
+        <v>0.918407740366541</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4429220015406774</v>
+        <v>0.3327546706147455</v>
       </c>
       <c r="H11" t="n">
-        <v>1.399026994896801</v>
+        <v>1.723423817978588</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4006557431132247</v>
+        <v>0.7591380967517685</v>
       </c>
       <c r="J11" t="n">
-        <v>0.3865195345366451</v>
+        <v>0.4649517542450144</v>
       </c>
       <c r="K11" t="n">
-        <v>0.3935876388249349</v>
+        <v>0.6120449254983914</v>
       </c>
       <c r="L11" t="n">
-        <v>1.793579735427304</v>
+        <v>0.7000979867819673</v>
       </c>
       <c r="M11" t="n">
-        <v>0.6655238549749193</v>
+        <v>0.5768489148943122</v>
       </c>
       <c r="N11" t="n">
-        <v>1.317933923051315</v>
+        <v>1.238854691061171</v>
       </c>
       <c r="O11" t="n">
-        <v>0.6938565833055045</v>
+        <v>0.6014065674432345</v>
       </c>
       <c r="P11" t="n">
-        <v>59.62872318639172</v>
+        <v>60.20069957079495</v>
       </c>
       <c r="Q11" t="n">
-        <v>94.97612210756954</v>
+        <v>95.54809849197277</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_2</t>
+          <t>model_11_7_11</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9320360587148523</v>
+        <v>0.9494820095122185</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7899170848862219</v>
+        <v>0.7422436179628001</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9144856661260906</v>
+        <v>0.9480658286795124</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9842851329736826</v>
+        <v>0.7108503765706558</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9559769281721932</v>
+        <v>0.9290208975806209</v>
       </c>
       <c r="G12" t="n">
-        <v>0.4544751883189571</v>
+        <v>0.337814035005752</v>
       </c>
       <c r="H12" t="n">
-        <v>1.404825420708711</v>
+        <v>1.723618113541763</v>
       </c>
       <c r="I12" t="n">
-        <v>0.3388775445251595</v>
+        <v>0.7106402061671305</v>
       </c>
       <c r="J12" t="n">
-        <v>0.08554676579867121</v>
+        <v>0.3542254967162085</v>
       </c>
       <c r="K12" t="n">
-        <v>0.2122121551619154</v>
+        <v>0.5324328514416695</v>
       </c>
       <c r="L12" t="n">
-        <v>1.708272760388153</v>
+        <v>0.7051906649019635</v>
       </c>
       <c r="M12" t="n">
-        <v>0.6741477496209248</v>
+        <v>0.5812177173880301</v>
       </c>
       <c r="N12" t="n">
-        <v>1.326226918168709</v>
+        <v>1.242486354341351</v>
       </c>
       <c r="O12" t="n">
-        <v>0.7028476150005134</v>
+        <v>0.6059613589037778</v>
       </c>
       <c r="P12" t="n">
-        <v>59.57722391602433</v>
+        <v>60.17051945440222</v>
       </c>
       <c r="Q12" t="n">
-        <v>94.92462283720215</v>
+        <v>95.51791837558004</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_13</t>
+          <t>model_11_7_22</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9330814221216388</v>
+        <v>0.950237526525031</v>
       </c>
       <c r="C13" t="n">
-        <v>0.7898103165706228</v>
+        <v>0.7422091892377849</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8906921742655983</v>
+        <v>0.9441571469235418</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9226079467066464</v>
+        <v>0.6105798165412759</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9113713404635042</v>
+        <v>0.9172680904960516</v>
       </c>
       <c r="G13" t="n">
-        <v>0.44748483840432</v>
+        <v>0.3327618892622389</v>
       </c>
       <c r="H13" t="n">
-        <v>1.405539380926745</v>
+        <v>1.723848338584469</v>
       </c>
       <c r="I13" t="n">
-        <v>0.4331667675371988</v>
+        <v>0.7641245756733573</v>
       </c>
       <c r="J13" t="n">
-        <v>0.4212978605976978</v>
+        <v>0.4770629001033121</v>
       </c>
       <c r="K13" t="n">
-        <v>0.4272323140674483</v>
+        <v>0.6205937378883346</v>
       </c>
       <c r="L13" t="n">
-        <v>1.798506809978639</v>
+        <v>0.6994790300130002</v>
       </c>
       <c r="M13" t="n">
-        <v>0.6689430756083211</v>
+        <v>0.5768551718258569</v>
       </c>
       <c r="N13" t="n">
-        <v>1.321209173816134</v>
+        <v>1.238859872679851</v>
       </c>
       <c r="O13" t="n">
-        <v>0.6974213672400327</v>
+        <v>0.6014130907453087</v>
       </c>
       <c r="P13" t="n">
-        <v>59.60822524500385</v>
+        <v>60.20065618406093</v>
       </c>
       <c r="Q13" t="n">
-        <v>94.95562416618166</v>
+        <v>95.54805510523873</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_14</t>
+          <t>model_11_7_10</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.9323113912175374</v>
+        <v>0.9493159940684111</v>
       </c>
       <c r="C14" t="n">
-        <v>0.7887037799555704</v>
+        <v>0.7421619467086573</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8813830987755089</v>
+        <v>0.9484070951118064</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9164900410474459</v>
+        <v>0.7187534796511335</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9040905142646504</v>
+        <v>0.9299775022077723</v>
       </c>
       <c r="G14" t="n">
-        <v>0.4526340386057124</v>
+        <v>0.3389241810429233</v>
       </c>
       <c r="H14" t="n">
-        <v>1.412938796366733</v>
+        <v>1.724164249594277</v>
       </c>
       <c r="I14" t="n">
-        <v>0.4700569180063859</v>
+        <v>0.7059704936900253</v>
       </c>
       <c r="J14" t="n">
-        <v>0.4546018040373407</v>
+        <v>0.3445437251092477</v>
       </c>
       <c r="K14" t="n">
-        <v>0.4623293610218633</v>
+        <v>0.5252571093996365</v>
       </c>
       <c r="L14" t="n">
-        <v>1.801566170614776</v>
+        <v>0.7055726715637021</v>
       </c>
       <c r="M14" t="n">
-        <v>0.6727808250877194</v>
+        <v>0.582171951439541</v>
       </c>
       <c r="N14" t="n">
-        <v>1.324905322155821</v>
+        <v>1.243283228471627</v>
       </c>
       <c r="O14" t="n">
-        <v>0.7014224976600055</v>
+        <v>0.6069562166743984</v>
       </c>
       <c r="P14" t="n">
-        <v>59.58534268358569</v>
+        <v>60.16395770271355</v>
       </c>
       <c r="Q14" t="n">
-        <v>94.93274160476351</v>
+        <v>95.51135662389137</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_1</t>
+          <t>model_11_7_23</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9308560183431278</v>
+        <v>0.9502247216792888</v>
       </c>
       <c r="C15" t="n">
-        <v>0.7886466085826762</v>
+        <v>0.7421356480052337</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9102935366473786</v>
+        <v>0.9437914948062586</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9872172290219364</v>
+        <v>0.6005857390020354</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9559093795532563</v>
+        <v>0.9161185017318535</v>
       </c>
       <c r="G15" t="n">
-        <v>0.462366123718265</v>
+        <v>0.3328475153246779</v>
       </c>
       <c r="H15" t="n">
-        <v>1.413321101600526</v>
+        <v>1.724340109145166</v>
       </c>
       <c r="I15" t="n">
-        <v>0.3554901810238801</v>
+        <v>0.7691279691887379</v>
       </c>
       <c r="J15" t="n">
-        <v>0.06958536227428182</v>
+        <v>0.4893062398613625</v>
       </c>
       <c r="K15" t="n">
-        <v>0.212537771649081</v>
+        <v>0.6292171045250502</v>
       </c>
       <c r="L15" t="n">
-        <v>1.697705118900542</v>
+        <v>0.6988442165050283</v>
       </c>
       <c r="M15" t="n">
-        <v>0.6799750905130754</v>
+        <v>0.5769293850417726</v>
       </c>
       <c r="N15" t="n">
-        <v>1.331891111952987</v>
+        <v>1.238921335939414</v>
       </c>
       <c r="O15" t="n">
-        <v>0.7089230378587014</v>
+        <v>0.6014904633714685</v>
       </c>
       <c r="P15" t="n">
-        <v>59.54279645232543</v>
+        <v>60.20014161162657</v>
       </c>
       <c r="Q15" t="n">
-        <v>94.89019537350325</v>
+        <v>95.54754053280439</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_15</t>
+          <t>model_11_7_9</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9314883478034186</v>
+        <v>0.9491307672150188</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7874960121693414</v>
+        <v>0.7420634213469317</v>
       </c>
       <c r="D16" t="n">
-        <v>0.871177893226514</v>
+        <v>0.9487453630032998</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9107545836342995</v>
+        <v>0.726387111839264</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8966572891103725</v>
+        <v>0.9309093677744555</v>
       </c>
       <c r="G16" t="n">
-        <v>0.4581377337056906</v>
+        <v>0.3401627938644486</v>
       </c>
       <c r="H16" t="n">
-        <v>1.421015145114505</v>
+        <v>1.724823089141804</v>
       </c>
       <c r="I16" t="n">
-        <v>0.5104982667388362</v>
+        <v>0.7013418116866658</v>
       </c>
       <c r="J16" t="n">
-        <v>0.4858238201860621</v>
+        <v>0.3351920713822972</v>
       </c>
       <c r="K16" t="n">
-        <v>0.4981610434624492</v>
+        <v>0.5182669415344815</v>
       </c>
       <c r="L16" t="n">
-        <v>1.802828324058133</v>
+        <v>0.7059263256462232</v>
       </c>
       <c r="M16" t="n">
-        <v>0.6768587250717025</v>
+        <v>0.5832347673659799</v>
       </c>
       <c r="N16" t="n">
-        <v>1.328855930543591</v>
+        <v>1.24417231736791</v>
       </c>
       <c r="O16" t="n">
-        <v>0.7056740022887236</v>
+        <v>0.608064278875158</v>
       </c>
       <c r="P16" t="n">
-        <v>59.56117082292538</v>
+        <v>60.15666194095805</v>
       </c>
       <c r="Q16" t="n">
-        <v>94.9085697441032</v>
+        <v>95.50406086213587</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_0</t>
+          <t>model_11_7_24</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9294805666141054</v>
+        <v>0.9502006168198031</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7871548144647577</v>
+        <v>0.7420523961380669</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9051927114606479</v>
+        <v>0.9434246442106056</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9894961759361213</v>
+        <v>0.5904919113994218</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9550995254932948</v>
+        <v>0.9149596745810292</v>
       </c>
       <c r="G17" t="n">
-        <v>0.4715637757636105</v>
+        <v>0.3330087046310521</v>
       </c>
       <c r="H17" t="n">
-        <v>1.423296735736128</v>
+        <v>1.72489681476425</v>
       </c>
       <c r="I17" t="n">
-        <v>0.3757038111374012</v>
+        <v>0.7741477620591888</v>
       </c>
       <c r="J17" t="n">
-        <v>0.05717949605798577</v>
+        <v>0.5016717793834198</v>
       </c>
       <c r="K17" t="n">
-        <v>0.2164416535976935</v>
+        <v>0.6379097707213043</v>
       </c>
       <c r="L17" t="n">
-        <v>1.687128916534067</v>
+        <v>0.6981952754227304</v>
       </c>
       <c r="M17" t="n">
-        <v>0.6867050136438575</v>
+        <v>0.5770690640045194</v>
       </c>
       <c r="N17" t="n">
-        <v>1.338493280252294</v>
+        <v>1.239037039264945</v>
       </c>
       <c r="O17" t="n">
-        <v>0.7159394677500224</v>
+        <v>0.6016360887568347</v>
       </c>
       <c r="P17" t="n">
-        <v>59.50340184925395</v>
+        <v>60.19917329862029</v>
       </c>
       <c r="Q17" t="n">
-        <v>94.85080077043176</v>
+        <v>95.54657221979811</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_16</t>
+          <t>model_11_7_8</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9306529860518671</v>
+        <v>0.9489254660733596</v>
       </c>
       <c r="C18" t="n">
-        <v>0.7862242919192862</v>
+        <v>0.741947349148526</v>
       </c>
       <c r="D18" t="n">
-        <v>0.8603592715017122</v>
+        <v>0.9490805176364404</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9055024931148052</v>
+        <v>0.7337333768317869</v>
       </c>
       <c r="F18" t="n">
-        <v>0.8892448545632712</v>
+        <v>0.9318149282927368</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4637238015848033</v>
+        <v>0.3415356435440484</v>
       </c>
       <c r="H18" t="n">
-        <v>1.429519144282358</v>
+        <v>1.725599264467007</v>
       </c>
       <c r="I18" t="n">
-        <v>0.5533704707210733</v>
+        <v>0.6967557298924055</v>
       </c>
       <c r="J18" t="n">
-        <v>0.5144145398448519</v>
+        <v>0.3261924595719045</v>
       </c>
       <c r="K18" t="n">
-        <v>0.5338925052829625</v>
+        <v>0.511474094732155</v>
       </c>
       <c r="L18" t="n">
-        <v>1.802236818077328</v>
+        <v>0.7062498285923807</v>
       </c>
       <c r="M18" t="n">
-        <v>0.6809726878405647</v>
+        <v>0.5844105094401095</v>
       </c>
       <c r="N18" t="n">
-        <v>1.332865666951038</v>
+        <v>1.245157762847874</v>
       </c>
       <c r="O18" t="n">
-        <v>0.7099631049697332</v>
+        <v>0.609290074723505</v>
       </c>
       <c r="P18" t="n">
-        <v>59.53693231839153</v>
+        <v>60.14860646387197</v>
       </c>
       <c r="Q18" t="n">
-        <v>94.88433123956933</v>
+        <v>95.49600538504978</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_17</t>
+          <t>model_11_7_7</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.9298476362694527</v>
+        <v>0.9486993042915473</v>
       </c>
       <c r="C19" t="n">
-        <v>0.7849283798165613</v>
+        <v>0.74181296039848</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8492578992334462</v>
+        <v>0.9494122067709173</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9008162897430101</v>
+        <v>0.7407743394225078</v>
       </c>
       <c r="F19" t="n">
-        <v>0.8820357217666024</v>
+        <v>0.9326923979585808</v>
       </c>
       <c r="G19" t="n">
-        <v>0.4691091792881034</v>
+        <v>0.3430479884204067</v>
       </c>
       <c r="H19" t="n">
-        <v>1.438184914480406</v>
+        <v>1.726497922657367</v>
       </c>
       <c r="I19" t="n">
-        <v>0.5973631629950581</v>
+        <v>0.6922170681805714</v>
       </c>
       <c r="J19" t="n">
-        <v>0.5399247488501551</v>
+        <v>0.3175668613730266</v>
       </c>
       <c r="K19" t="n">
-        <v>0.5686439559226065</v>
+        <v>0.504891964776799</v>
       </c>
       <c r="L19" t="n">
-        <v>1.79959276794815</v>
+        <v>0.7065459646880037</v>
       </c>
       <c r="M19" t="n">
-        <v>0.6849154541168592</v>
+        <v>0.5857029865216726</v>
       </c>
       <c r="N19" t="n">
-        <v>1.336731345906627</v>
+        <v>1.246243339400573</v>
       </c>
       <c r="O19" t="n">
-        <v>0.7140737229690608</v>
+        <v>0.6106375752302267</v>
       </c>
       <c r="P19" t="n">
-        <v>59.51383949193713</v>
+        <v>60.13976986734237</v>
       </c>
       <c r="Q19" t="n">
-        <v>94.86123841311493</v>
+        <v>95.48716878852018</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_18</t>
+          <t>model_11_7_6</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.9291136510652487</v>
+        <v>0.9484514220056283</v>
       </c>
       <c r="C20" t="n">
-        <v>0.7836484051850848</v>
+        <v>0.741659454270889</v>
       </c>
       <c r="D20" t="n">
-        <v>0.8382242379589655</v>
+        <v>0.9497404659929797</v>
       </c>
       <c r="E20" t="n">
-        <v>0.896755972657531</v>
+        <v>0.7474903319605104</v>
       </c>
       <c r="F20" t="n">
-        <v>0.8752078224083981</v>
+        <v>0.9335402032301774</v>
       </c>
       <c r="G20" t="n">
-        <v>0.4740173417283067</v>
+        <v>0.3447055784077402</v>
       </c>
       <c r="H20" t="n">
-        <v>1.44674411073483</v>
+        <v>1.727524418839399</v>
       </c>
       <c r="I20" t="n">
-        <v>0.6410875290800654</v>
+        <v>0.6877253396074302</v>
       </c>
       <c r="J20" t="n">
-        <v>0.562027830867847</v>
+        <v>0.3093393708285072</v>
       </c>
       <c r="K20" t="n">
-        <v>0.6015576799739561</v>
+        <v>0.4985323552179686</v>
       </c>
       <c r="L20" t="n">
-        <v>1.794898221234501</v>
+        <v>0.7068099106733122</v>
       </c>
       <c r="M20" t="n">
-        <v>0.688489173283289</v>
+        <v>0.5871163244262079</v>
       </c>
       <c r="N20" t="n">
-        <v>1.340254474886806</v>
+        <v>1.247433174372984</v>
       </c>
       <c r="O20" t="n">
-        <v>0.7177995827590241</v>
+        <v>0.6121110818553708</v>
       </c>
       <c r="P20" t="n">
-        <v>59.49302274406323</v>
+        <v>60.13012924443995</v>
       </c>
       <c r="Q20" t="n">
-        <v>94.84042166524104</v>
+        <v>95.47752816561776</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_19</t>
+          <t>model_11_7_5</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.9284873106201902</v>
+        <v>0.948180951314337</v>
       </c>
       <c r="C21" t="n">
-        <v>0.7824217785157064</v>
+        <v>0.7414860468004343</v>
       </c>
       <c r="D21" t="n">
-        <v>0.8275887927037696</v>
+        <v>0.9500650602554396</v>
       </c>
       <c r="E21" t="n">
-        <v>0.8933557297466108</v>
+        <v>0.7538584426138544</v>
       </c>
       <c r="F21" t="n">
-        <v>0.8689163111451578</v>
+        <v>0.9343562588170274</v>
       </c>
       <c r="G21" t="n">
-        <v>0.4782056831684453</v>
+        <v>0.3465142171658083</v>
       </c>
       <c r="H21" t="n">
-        <v>1.454946568921061</v>
+        <v>1.728683995392798</v>
       </c>
       <c r="I21" t="n">
-        <v>0.6832338384733746</v>
+        <v>0.6832837604365283</v>
       </c>
       <c r="J21" t="n">
-        <v>0.5805376778472682</v>
+        <v>0.301538056296013</v>
       </c>
       <c r="K21" t="n">
-        <v>0.6318857581603214</v>
+        <v>0.4924109083662707</v>
       </c>
       <c r="L21" t="n">
-        <v>1.788197958779197</v>
+        <v>0.7070426921646196</v>
       </c>
       <c r="M21" t="n">
-        <v>0.6915241739581092</v>
+        <v>0.5886545822176265</v>
       </c>
       <c r="N21" t="n">
-        <v>1.343260909023087</v>
+        <v>1.248731433691182</v>
       </c>
       <c r="O21" t="n">
-        <v>0.7209637896958889</v>
+        <v>0.6137148264656026</v>
       </c>
       <c r="P21" t="n">
-        <v>59.47542867905479</v>
+        <v>60.11966286082473</v>
       </c>
       <c r="Q21" t="n">
-        <v>94.8228276002326</v>
+        <v>95.46706178200255</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_20</t>
+          <t>model_11_7_4</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.9279971024550188</v>
+        <v>0.9478868014417465</v>
       </c>
       <c r="C22" t="n">
-        <v>0.7812800679926883</v>
+        <v>0.7412918838197392</v>
       </c>
       <c r="D22" t="n">
-        <v>0.8176371878254967</v>
+        <v>0.9503857608162096</v>
       </c>
       <c r="E22" t="n">
-        <v>0.8906247044827507</v>
+        <v>0.759857563135143</v>
       </c>
       <c r="F22" t="n">
-        <v>0.8632837537664054</v>
+        <v>0.9351386324544883</v>
       </c>
       <c r="G22" t="n">
-        <v>0.4814837074261474</v>
+        <v>0.3484811987182564</v>
       </c>
       <c r="H22" t="n">
-        <v>1.462581192445576</v>
+        <v>1.729982364138744</v>
       </c>
       <c r="I22" t="n">
-        <v>0.7226702144873224</v>
+        <v>0.6788954606556924</v>
       </c>
       <c r="J22" t="n">
-        <v>0.5954045156160159</v>
+        <v>0.2941887766348098</v>
       </c>
       <c r="K22" t="n">
-        <v>0.6590373650516691</v>
+        <v>0.4865421186452511</v>
       </c>
       <c r="L22" t="n">
-        <v>1.779592551047614</v>
+        <v>0.7072455223418301</v>
       </c>
       <c r="M22" t="n">
-        <v>0.6938902704507013</v>
+        <v>0.5903229613679756</v>
       </c>
       <c r="N22" t="n">
-        <v>1.34561390821591</v>
+        <v>1.250143353079617</v>
       </c>
       <c r="O22" t="n">
-        <v>0.7234306158146656</v>
+        <v>0.6154542319704031</v>
       </c>
       <c r="P22" t="n">
-        <v>59.46176577087527</v>
+        <v>60.10834199879077</v>
       </c>
       <c r="Q22" t="n">
-        <v>94.80916469205309</v>
+        <v>95.45574091996858</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_21</t>
+          <t>model_11_7_3</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.9276619346652974</v>
+        <v>0.9475681591257801</v>
       </c>
       <c r="C23" t="n">
-        <v>0.7802477061373689</v>
+        <v>0.7410760442699234</v>
       </c>
       <c r="D23" t="n">
-        <v>0.8085859594886589</v>
+        <v>0.950702359272566</v>
       </c>
       <c r="E23" t="n">
-        <v>0.8885482585610218</v>
+        <v>0.7654639431497018</v>
       </c>
       <c r="F23" t="n">
-        <v>0.8583908898745591</v>
+        <v>0.9358851946811096</v>
       </c>
       <c r="G23" t="n">
-        <v>0.4837249759793194</v>
+        <v>0.3506119613523371</v>
       </c>
       <c r="H23" t="n">
-        <v>1.469484600925685</v>
+        <v>1.731425684202212</v>
       </c>
       <c r="I23" t="n">
-        <v>0.7585385642103849</v>
+        <v>0.6745632919394766</v>
       </c>
       <c r="J23" t="n">
-        <v>0.6067080304763234</v>
+        <v>0.2873206274673176</v>
       </c>
       <c r="K23" t="n">
-        <v>0.682623297343354</v>
+        <v>0.4809419597033971</v>
       </c>
       <c r="L23" t="n">
-        <v>1.769216931996671</v>
+        <v>0.7074141544621892</v>
       </c>
       <c r="M23" t="n">
-        <v>0.6955033975325494</v>
+        <v>0.5921249541712772</v>
       </c>
       <c r="N23" t="n">
-        <v>1.347222713606572</v>
+        <v>1.251672836196256</v>
       </c>
       <c r="O23" t="n">
-        <v>0.7251124170560214</v>
+        <v>0.6173329393379805</v>
       </c>
       <c r="P23" t="n">
-        <v>59.45247753043573</v>
+        <v>60.09615038054106</v>
       </c>
       <c r="Q23" t="n">
-        <v>94.79987645161354</v>
+        <v>95.44354930171887</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_22</t>
+          <t>model_11_7_2</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9274905216022529</v>
+        <v>0.9472239405291036</v>
       </c>
       <c r="C24" t="n">
-        <v>0.7793399612445706</v>
+        <v>0.7408376593836699</v>
       </c>
       <c r="D24" t="n">
-        <v>0.8005730385311864</v>
+        <v>0.9510148185438527</v>
       </c>
       <c r="E24" t="n">
-        <v>0.8870901185226371</v>
+        <v>0.7706543687377925</v>
       </c>
       <c r="F24" t="n">
-        <v>0.854273933036741</v>
+        <v>0.9365940160998649</v>
       </c>
       <c r="G24" t="n">
-        <v>0.484871215921183</v>
+        <v>0.3529137526932932</v>
       </c>
       <c r="H24" t="n">
-        <v>1.475554695203609</v>
+        <v>1.733019765034251</v>
       </c>
       <c r="I24" t="n">
-        <v>0.790292293153024</v>
+        <v>0.6702877616802985</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6146456836652731</v>
+        <v>0.2809620472267342</v>
       </c>
       <c r="K24" t="n">
-        <v>0.7024689884091486</v>
+        <v>0.4756249044535162</v>
       </c>
       <c r="L24" t="n">
-        <v>1.757237992500358</v>
+        <v>0.7075425733345878</v>
       </c>
       <c r="M24" t="n">
-        <v>0.6963269461403767</v>
+        <v>0.5940654447897918</v>
       </c>
       <c r="N24" t="n">
-        <v>1.348045496309186</v>
+        <v>1.253325085460303</v>
       </c>
       <c r="O24" t="n">
-        <v>0.7259710258330645</v>
+        <v>0.6193560406594947</v>
       </c>
       <c r="P24" t="n">
-        <v>59.44774391497645</v>
+        <v>60.08306315709871</v>
       </c>
       <c r="Q24" t="n">
-        <v>94.79514283615427</v>
+        <v>95.43046207827652</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_23</t>
+          <t>model_11_7_1</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9274825177117788</v>
+        <v>0.9468530439517505</v>
       </c>
       <c r="C25" t="n">
-        <v>0.7785643048247095</v>
+        <v>0.7405757489069711</v>
       </c>
       <c r="D25" t="n">
-        <v>0.7936613546816941</v>
+        <v>0.9513227248638303</v>
       </c>
       <c r="E25" t="n">
-        <v>0.8861994654839158</v>
+        <v>0.7754014311926727</v>
       </c>
       <c r="F25" t="n">
-        <v>0.8509300554187045</v>
+        <v>0.9372624812136208</v>
       </c>
       <c r="G25" t="n">
-        <v>0.4849247379736379</v>
+        <v>0.3553939398138751</v>
       </c>
       <c r="H25" t="n">
-        <v>1.480741513254789</v>
+        <v>1.734771161597923</v>
       </c>
       <c r="I25" t="n">
-        <v>0.8176820223989274</v>
+        <v>0.6660745316403163</v>
       </c>
       <c r="J25" t="n">
-        <v>0.6194941171126429</v>
+        <v>0.2751466132099797</v>
       </c>
       <c r="K25" t="n">
-        <v>0.7185880697557852</v>
+        <v>0.470610572425148</v>
       </c>
       <c r="L25" t="n">
-        <v>1.743842111998006</v>
+        <v>0.7076395331033257</v>
       </c>
       <c r="M25" t="n">
-        <v>0.6963653767769029</v>
+        <v>0.596149259677369</v>
       </c>
       <c r="N25" t="n">
-        <v>1.348083914983462</v>
+        <v>1.255105389031598</v>
       </c>
       <c r="O25" t="n">
-        <v>0.72601109254135</v>
+        <v>0.6215285678609275</v>
       </c>
       <c r="P25" t="n">
-        <v>59.44752315904405</v>
+        <v>60.06905683028116</v>
       </c>
       <c r="Q25" t="n">
-        <v>94.79492208022187</v>
+        <v>95.41645575145897</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_24</t>
+          <t>model_11_7_0</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.9276301434536878</v>
+        <v>0.9464544231224331</v>
       </c>
       <c r="C26" t="n">
-        <v>0.7779208780924772</v>
+        <v>0.7402893112758393</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7878491606679391</v>
+        <v>0.9516262094513415</v>
       </c>
       <c r="E26" t="n">
-        <v>0.885815799450242</v>
+        <v>0.779677293370216</v>
       </c>
       <c r="F26" t="n">
-        <v>0.8483243779998714</v>
+        <v>0.937888436609571</v>
       </c>
       <c r="G26" t="n">
-        <v>0.4839375639577383</v>
+        <v>0.3580595191350007</v>
       </c>
       <c r="H26" t="n">
-        <v>1.485044110775935</v>
+        <v>1.736686571356225</v>
       </c>
       <c r="I26" t="n">
-        <v>0.8407146760659644</v>
+        <v>0.6619218062890914</v>
       </c>
       <c r="J26" t="n">
-        <v>0.6215826736542052</v>
+        <v>0.2699084275752665</v>
       </c>
       <c r="K26" t="n">
-        <v>0.7311486748600848</v>
+        <v>0.465915116932179</v>
       </c>
       <c r="L26" t="n">
-        <v>1.729224729774439</v>
+        <v>0.7076951206715837</v>
       </c>
       <c r="M26" t="n">
-        <v>0.6956562110394316</v>
+        <v>0.5983807476306375</v>
       </c>
       <c r="N26" t="n">
-        <v>1.347375311422299</v>
+        <v>1.257018769012321</v>
       </c>
       <c r="O26" t="n">
-        <v>0.7252717361502592</v>
+        <v>0.6238550548761835</v>
       </c>
       <c r="P26" t="n">
-        <v>59.4515987613481</v>
+        <v>60.05411210366631</v>
       </c>
       <c r="Q26" t="n">
-        <v>94.79899768252591</v>
+        <v>95.40151102484413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>